<commit_message>
updated test case plan ith Sam's tests
</commit_message>
<xml_diff>
--- a/Group1 Test Case Plan.xlsx
+++ b/Group1 Test Case Plan.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9084"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9084"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="50">
   <si>
     <t>Scenario</t>
   </si>
@@ -120,6 +120,60 @@
   </si>
   <si>
     <t>Test resetting a racer at the start</t>
+  </si>
+  <si>
+    <t>testNewRacer</t>
+  </si>
+  <si>
+    <t>Sprint 2</t>
+  </si>
+  <si>
+    <t>Ran - Passed</t>
+  </si>
+  <si>
+    <t>testRacerStartFinish</t>
+  </si>
+  <si>
+    <t>Test creation of a Racer and associated getters</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test starting and stoping a Racer and associated getters </t>
+  </si>
+  <si>
+    <t>Tester</t>
+  </si>
+  <si>
+    <t>Sam</t>
+  </si>
+  <si>
+    <t>testNewStartSensor</t>
+  </si>
+  <si>
+    <t>testNewStopSensor</t>
+  </si>
+  <si>
+    <t>TestToggleSensor</t>
+  </si>
+  <si>
+    <t>merge with stopsensor?</t>
+  </si>
+  <si>
+    <t>merge with startsensor?</t>
+  </si>
+  <si>
+    <t>Test adding a Sensor to a start trigger</t>
+  </si>
+  <si>
+    <t>Test adding a Sensor to a stop trigger</t>
+  </si>
+  <si>
+    <t>merge with other sensors?</t>
+  </si>
+  <si>
+    <t>Test ability to toggle a Sensor on and off</t>
+  </si>
+  <si>
+    <t>Functional Tests</t>
   </si>
 </sst>
 </file>
@@ -490,10 +544,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:J8"/>
+  <dimension ref="B1:J15"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="B2" sqref="A2:XFD7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -502,9 +556,9 @@
     <col min="2" max="2" width="14.6640625" customWidth="1"/>
     <col min="3" max="3" width="0" hidden="1" customWidth="1"/>
     <col min="4" max="4" width="18" customWidth="1"/>
-    <col min="5" max="5" width="33.21875" customWidth="1"/>
-    <col min="6" max="6" width="14.109375" customWidth="1"/>
-    <col min="7" max="7" width="0" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="34" style="1" customWidth="1"/>
+    <col min="6" max="6" width="8.88671875" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="14.109375" customWidth="1"/>
     <col min="8" max="8" width="22.88671875" customWidth="1"/>
     <col min="9" max="9" width="11" customWidth="1"/>
     <col min="10" max="10" width="30.21875" customWidth="1"/>
@@ -522,9 +576,11 @@
         <v>2</v>
       </c>
       <c r="F1" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="3"/>
       <c r="H1" s="3" t="s">
         <v>4</v>
       </c>
@@ -535,7 +591,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="2:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:10" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>29</v>
       </c>
@@ -545,7 +601,7 @@
       <c r="E2" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>8</v>
       </c>
       <c r="H2" s="1"/>
@@ -556,17 +612,17 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="2:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:10" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>29</v>
       </c>
       <c r="D3" t="s">
         <v>22</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>8</v>
       </c>
       <c r="H3" s="1"/>
@@ -577,7 +633,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="2:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:10" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="B4" s="1" t="s">
         <v>12</v>
       </c>
@@ -588,10 +644,10 @@
       <c r="E4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="F4" s="1"/>
+      <c r="G4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="1"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1" t="s">
         <v>17</v>
@@ -600,7 +656,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="2:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:10" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="B5" s="1" t="s">
         <v>12</v>
       </c>
@@ -611,10 +667,10 @@
       <c r="E5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="F5" s="1"/>
+      <c r="G5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G5" s="1"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1" t="s">
         <v>17</v>
@@ -623,7 +679,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="2:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:10" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="B6" s="1" t="s">
         <v>13</v>
       </c>
@@ -634,10 +690,10 @@
       <c r="E6" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="F6" s="1"/>
+      <c r="G6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G6" s="1"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1" t="s">
         <v>18</v>
@@ -646,7 +702,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="2:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:10" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="B7" s="1" t="s">
         <v>15</v>
       </c>
@@ -657,10 +713,10 @@
       <c r="E7" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="F7" s="1"/>
+      <c r="G7" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G7" s="1"/>
       <c r="H7" s="1"/>
       <c r="I7" s="1" t="s">
         <v>18</v>
@@ -673,15 +729,99 @@
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1" t="s">
-        <v>8</v>
-      </c>
+      <c r="F8" s="1"/>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
     </row>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B9" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="11" spans="2:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="D11" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F11" t="s">
+        <v>39</v>
+      </c>
+      <c r="G11" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="2:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="D12" t="s">
+        <v>35</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F12" t="s">
+        <v>39</v>
+      </c>
+      <c r="G12" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="D13" t="s">
+        <v>40</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F13" t="s">
+        <v>39</v>
+      </c>
+      <c r="G13" t="s">
+        <v>34</v>
+      </c>
+      <c r="H13" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="14" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="D14" t="s">
+        <v>41</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F14" t="s">
+        <v>39</v>
+      </c>
+      <c r="G14" t="s">
+        <v>34</v>
+      </c>
+      <c r="H14" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="15" spans="2:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="D15" t="s">
+        <v>42</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F15" t="s">
+        <v>39</v>
+      </c>
+      <c r="G15" t="s">
+        <v>34</v>
+      </c>
+      <c r="H15" t="s">
+        <v>47</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
moved pics to folder Models
</commit_message>
<xml_diff>
--- a/Group1 Test Case Plan.xlsx
+++ b/Group1 Test Case Plan.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9084"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9084"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="57">
   <si>
     <t>Scenario</t>
   </si>
@@ -174,6 +174,27 @@
   </si>
   <si>
     <t>Functional Tests</t>
+  </si>
+  <si>
+    <t>TestLane</t>
+  </si>
+  <si>
+    <t>Test Lane class functionality</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Handle multiple Racers at once, DNF cases, SWAP cases, </t>
+  </si>
+  <si>
+    <t>Default toggle off</t>
+  </si>
+  <si>
+    <t>Associate a specific trigger to a sensor</t>
+  </si>
+  <si>
+    <t>Racers has a Bib number</t>
+  </si>
+  <si>
+    <t>Racer knows own time info</t>
   </si>
 </sst>
 </file>
@@ -544,10 +565,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:J15"/>
+  <dimension ref="B1:J16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B2" sqref="A2:XFD7"/>
+    <sheetView tabSelected="1" topLeftCell="D8" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -556,12 +577,12 @@
     <col min="2" max="2" width="14.6640625" customWidth="1"/>
     <col min="3" max="3" width="0" hidden="1" customWidth="1"/>
     <col min="4" max="4" width="18" customWidth="1"/>
-    <col min="5" max="5" width="34" style="1" customWidth="1"/>
-    <col min="6" max="6" width="8.88671875" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="33.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14.109375" customWidth="1"/>
     <col min="8" max="8" width="22.88671875" customWidth="1"/>
     <col min="9" max="9" width="11" customWidth="1"/>
-    <col min="10" max="10" width="30.21875" customWidth="1"/>
+    <col min="10" max="10" width="30.21875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -733,7 +754,6 @@
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
-      <c r="J8" s="1"/>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B9" s="1" t="s">
@@ -756,6 +776,9 @@
       <c r="G11" t="s">
         <v>34</v>
       </c>
+      <c r="J11" s="1" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="12" spans="2:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="D12" t="s">
@@ -770,8 +793,11 @@
       <c r="G12" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="J12" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="13" spans="2:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="D13" t="s">
         <v>40</v>
       </c>
@@ -787,8 +813,11 @@
       <c r="H13" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="J13" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="14" spans="2:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="D14" t="s">
         <v>41</v>
       </c>
@@ -803,6 +832,9 @@
       </c>
       <c r="H14" t="s">
         <v>44</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="15" spans="2:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -820,6 +852,26 @@
       </c>
       <c r="H15" t="s">
         <v>47</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="16" spans="2:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="D16" t="s">
+        <v>50</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F16" t="s">
+        <v>39</v>
+      </c>
+      <c r="G16" t="s">
+        <v>34</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
test case plan sheet
</commit_message>
<xml_diff>
--- a/Group1 Test Case Plan.xlsx
+++ b/Group1 Test Case Plan.xlsx
@@ -1,28 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="26221"/>
-  <workbookPr autoCompressPictures="0"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="164011"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jessica\Documents\GitHub\CS361_Final_Project\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22800" windowHeight="13600"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22800" windowHeight="13596"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="68">
   <si>
     <t>Scenario</t>
   </si>
@@ -186,12 +191,6 @@
     <t>testUpdateTime</t>
   </si>
   <si>
-    <t>Test ability to update time</t>
-  </si>
-  <si>
-    <t>Test a paragrpividual event</t>
-  </si>
-  <si>
     <t>Test a group event</t>
   </si>
   <si>
@@ -208,12 +207,36 @@
   </si>
   <si>
     <t>Test creation and sample run of a paraividual event</t>
+  </si>
+  <si>
+    <t>Sam/Jess</t>
+  </si>
+  <si>
+    <t>TestCLR</t>
+  </si>
+  <si>
+    <t>Test a paragr pividual event</t>
+  </si>
+  <si>
+    <t>Test CLR for IND events</t>
+  </si>
+  <si>
+    <t>Ran - Failed</t>
+  </si>
+  <si>
+    <t>Print function not overwritng old data</t>
+  </si>
+  <si>
+    <t>Jess</t>
+  </si>
+  <si>
+    <t>Test ability to update time between float and string formats</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -594,7 +617,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -602,27 +625,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:J19"/>
+  <dimension ref="B1:J20"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="0" hidden="1" customWidth="1"/>
     <col min="2" max="2" width="14.6640625" customWidth="1"/>
     <col min="3" max="3" width="0" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="19.5" customWidth="1"/>
+    <col min="4" max="4" width="19.44140625" customWidth="1"/>
     <col min="5" max="5" width="33.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.1640625" customWidth="1"/>
-    <col min="8" max="8" width="22.83203125" customWidth="1"/>
+    <col min="6" max="6" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.109375" customWidth="1"/>
+    <col min="8" max="8" width="24.6640625" customWidth="1"/>
     <col min="9" max="9" width="11" customWidth="1"/>
     <col min="10" max="10" width="30.33203125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" s="2" customFormat="1">
+    <row r="1" spans="2:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
@@ -649,7 +672,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="2:10" ht="28" hidden="1">
+    <row r="2" spans="2:10" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>29</v>
       </c>
@@ -670,7 +693,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="2:10" ht="28" hidden="1">
+    <row r="3" spans="2:10" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>29</v>
       </c>
@@ -691,7 +714,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="2:10" ht="28" hidden="1">
+    <row r="4" spans="2:10" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="B4" s="1" t="s">
         <v>12</v>
       </c>
@@ -714,7 +737,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="2:10" ht="28" hidden="1">
+    <row r="5" spans="2:10" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="B5" s="1" t="s">
         <v>12</v>
       </c>
@@ -737,7 +760,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="2:10" ht="28" hidden="1">
+    <row r="6" spans="2:10" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="B6" s="1" t="s">
         <v>13</v>
       </c>
@@ -760,7 +783,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="2:10" ht="28" hidden="1">
+    <row r="7" spans="2:10" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="B7" s="1" t="s">
         <v>15</v>
       </c>
@@ -783,7 +806,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="2:10">
+    <row r="8" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
@@ -792,7 +815,7 @@
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
     </row>
-    <row r="9" spans="2:10">
+    <row r="9" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B9" s="1" t="s">
         <v>33</v>
       </c>
@@ -800,7 +823,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="2:10" ht="28">
+    <row r="11" spans="2:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="D11" s="1" t="s">
         <v>32</v>
       </c>
@@ -817,7 +840,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="12" spans="2:10" ht="48" customHeight="1">
+    <row r="12" spans="2:10" ht="48" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D12" t="s">
         <v>52</v>
       </c>
@@ -831,13 +854,13 @@
         <v>34</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="J12" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="13" spans="2:10" ht="15.75" customHeight="1">
+    <row r="13" spans="2:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D13" t="s">
         <v>41</v>
       </c>
@@ -854,7 +877,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="14" spans="2:10" ht="28">
+    <row r="14" spans="2:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="D14" t="s">
         <v>35</v>
       </c>
@@ -868,18 +891,18 @@
         <v>34</v>
       </c>
       <c r="H14" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="J14" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="15" spans="2:10" ht="15.75" customHeight="1">
+    <row r="15" spans="2:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="D15" t="s">
         <v>53</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>54</v>
+        <v>67</v>
       </c>
       <c r="F15" t="s">
         <v>39</v>
@@ -888,54 +911,77 @@
         <v>34</v>
       </c>
     </row>
-    <row r="16" spans="2:10" ht="28">
+    <row r="16" spans="2:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="D16" t="s">
         <v>47</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F16" t="s">
-        <v>39</v>
+        <v>60</v>
       </c>
       <c r="G16" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="17" spans="4:7" ht="28">
+    <row r="17" spans="4:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="D17" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F17" t="s">
-        <v>39</v>
+        <v>60</v>
       </c>
       <c r="G17" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="18" spans="4:7">
+    <row r="18" spans="4:8" x14ac:dyDescent="0.3">
       <c r="D18" t="s">
         <v>48</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
+      </c>
+      <c r="F18" t="s">
+        <v>66</v>
       </c>
       <c r="G18" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="19" spans="4:7">
+    <row r="19" spans="4:8" x14ac:dyDescent="0.3">
       <c r="D19" t="s">
         <v>49</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>55</v>
+        <v>62</v>
+      </c>
+      <c r="F19" t="s">
+        <v>66</v>
       </c>
       <c r="G19" t="s">
         <v>50</v>
+      </c>
+    </row>
+    <row r="20" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="D20" t="s">
+        <v>61</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F20" t="s">
+        <v>66</v>
+      </c>
+      <c r="G20" t="s">
+        <v>64</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>